<commit_message>
Added Listerners and modified excel test data
</commit_message>
<xml_diff>
--- a/src/main/java/TestDataExcel/LoginUserNames.xlsx
+++ b/src/main/java/TestDataExcel/LoginUserNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse Workspace\Swag_Labs_Project_Page_Factory_June_2025\src\main\java\TestDataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C5579F-D727-4DAD-B95F-1450C78F1B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C01C2E-23B4-4D6E-9C42-143671B637F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EF150091-E94A-4267-AA70-EBC26E73EA2A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
   </si>
   <si>
     <t>problem_user</t>
@@ -406,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2752CF38-8E6B-4D48-9D88-6841C1966424}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -439,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -447,15 +444,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>